<commit_message>
All tokens for experiments
</commit_message>
<xml_diff>
--- a/ctl_properties.xlsx
+++ b/ctl_properties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/keerthi_nelaturu_mail_utoronto_ca/Documents/verisolid/verisolid_journal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Keerthi\Work\verisolid\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="459" documentId="8_{09F0B8C9-5966-8A41-9B70-03D7F00919D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0D77404E-45BC-4ECC-8E11-6033770825F6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B163AC00-D237-47DB-B267-A4A1C49395AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ERC20" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="163">
   <si>
     <t>Rule in Specification</t>
   </si>
@@ -528,6 +528,54 @@
   </si>
   <si>
     <t>AG(!T | (T &amp; !R -&gt;  !E[!Req U R]))</t>
+  </si>
+  <si>
+    <t>Transfer event is emitted when NFT is created or destroyed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Approval emits when there is a change in approved address: changed or reaffirmed </t>
+  </si>
+  <si>
+    <t>ApprovalForAll emitted when owner is enabled or disabled to manage the NFTs</t>
+  </si>
+  <si>
+    <t>safeTransferFrom throws if _from is not an owner</t>
+  </si>
+  <si>
+    <t>Throw if msg.sender is not the owner</t>
+  </si>
+  <si>
+    <t>Throw if msg.sender is not the authorized operator</t>
+  </si>
+  <si>
+    <t>Throw if _to is a zero address</t>
+  </si>
+  <si>
+    <t>Throws if _tokenId is not a valid NFT</t>
+  </si>
+  <si>
+    <t>If _to is a smart contract, onERC721Received is called and throws if return value is not bytes4(keccak256("onERC721Received(address,address,uint256,bytes)"))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">safeTransferFrom with data </t>
+  </si>
+  <si>
+    <t>Approve</t>
+  </si>
+  <si>
+    <t>Contract must allow multiple operators per owner</t>
+  </si>
+  <si>
+    <t>getApproved</t>
+  </si>
+  <si>
+    <t>onERC721Received</t>
+  </si>
+  <si>
+    <t>Contract address is always the msg.sender</t>
+  </si>
+  <si>
+    <t>Throw if msg.sender is not the owner or authorized operator or approved for the NFT</t>
   </si>
 </sst>
 </file>
@@ -768,7 +816,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -842,6 +890,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1159,7 +1210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29778301-1159-4B58-BDCD-90BA0F3971B0}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1315,7 +1366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B2CAF51-E601-49B8-9142-AF83A7AC00AB}">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -2175,7 +2226,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E0F917F-7C17-4DD6-9D54-EFA6449AB27E}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -2317,16 +2368,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C2FBDD6-E565-FE42-BA77-B53E83DF4184}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="3" width="37.125" customWidth="1"/>
+    <col min="2" max="2" width="37.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="37.125" customWidth="1"/>
     <col min="4" max="4" width="43.375" hidden="1" customWidth="1"/>
     <col min="5" max="6" width="43.375" customWidth="1"/>
     <col min="7" max="7" width="35.375" bestFit="1" customWidth="1"/>
@@ -2363,7 +2415,7 @@
       <c r="A2" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>144</v>
       </c>
       <c r="C2" s="7"/>
@@ -2374,7 +2426,7 @@
     </row>
     <row r="3" spans="1:8" ht="47.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="16" t="s">
         <v>145</v>
       </c>
       <c r="C3" s="7"/>
@@ -2383,52 +2435,124 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="31.5">
       <c r="A4" s="6"/>
-      <c r="B4" s="8"/>
+      <c r="B4" s="7" t="s">
+        <v>147</v>
+      </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="31.5">
       <c r="A5" s="11"/>
-      <c r="B5" s="9"/>
+      <c r="B5" s="9" t="s">
+        <v>148</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="31.5">
       <c r="A6" s="12"/>
-      <c r="B6" s="7"/>
+      <c r="B6" s="9" t="s">
+        <v>149</v>
+      </c>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+    <row r="7" spans="1:8" ht="31.5">
+      <c r="A7" s="7"/>
+      <c r="B7" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+    </row>
+    <row r="8" spans="1:8" ht="31.5">
+      <c r="A8" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="31.5">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="78.75">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="31.5">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="31.5">
+      <c r="A16" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>